<commit_message>
nhiem vu ngay 31/10
</commit_message>
<xml_diff>
--- a/BaoCaoHangNgay.xlsx
+++ b/BaoCaoHangNgay.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Ngày</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>Làm báo cáo</t>
+  </si>
+  <si>
+    <t>sửa lỗi giới tính ở trang đăng nhập</t>
+  </si>
+  <si>
+    <t>sửa lỗi đăng nhập ko thành công</t>
+  </si>
+  <si>
+    <t>sửa lỗi trang more-info ko hiện thông tin gì</t>
+  </si>
+  <si>
+    <t>làm cái bấm vào điểm đến yêu thích ra list các tour</t>
   </si>
 </sst>
 </file>
@@ -107,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -156,11 +168,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -173,6 +196,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -479,7 +505,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,20 +604,30 @@
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -641,7 +677,7 @@
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>